<commit_message>
Updated Grade doc for winter grades
</commit_message>
<xml_diff>
--- a/Year 4 Grades.xlsx
+++ b/Year 4 Grades.xlsx
@@ -1,32 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\University\Year 4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\University\Year 4\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B0326D-1ECB-444C-A08E-B930ED90CD8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D082FC1B-73E1-4252-9252-722FEC9A977F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="769" firstSheet="5" activeTab="11" xr2:uid="{A1BD24B9-1795-480B-9592-5AE2E18FE68C}"/>
+    <workbookView xWindow="-8745" yWindow="7950" windowWidth="18060" windowHeight="15435" tabRatio="769" activeTab="2" xr2:uid="{A1BD24B9-1795-480B-9592-5AE2E18FE68C}"/>
   </bookViews>
   <sheets>
-    <sheet name="SYSC 3303" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="SYSC 3320" sheetId="2" state="hidden" r:id="rId2"/>
-    <sheet name="SYSC 4001" sheetId="3" state="hidden" r:id="rId3"/>
-    <sheet name="SYSC 3501" sheetId="4" state="hidden" r:id="rId4"/>
-    <sheet name="TSES 4012" sheetId="5" state="hidden" r:id="rId5"/>
-    <sheet name="SYSC 4602" sheetId="7" r:id="rId6"/>
-    <sheet name="ELEC 4705" sheetId="6" r:id="rId7"/>
-    <sheet name="SYSC 4310" sheetId="8" r:id="rId8"/>
-    <sheet name="SYSC4810" sheetId="9" r:id="rId9"/>
-    <sheet name="SYSC4805" sheetId="10" r:id="rId10"/>
-    <sheet name="SYSC 4907" sheetId="11" r:id="rId11"/>
-    <sheet name="Transcript" sheetId="14" r:id="rId12"/>
-    <sheet name="Sheet1" sheetId="15" state="hidden" r:id="rId13"/>
-    <sheet name="LetterGrade Lookup" sheetId="12" state="hidden" r:id="rId14"/>
+    <sheet name="SYSC 4504" sheetId="1" r:id="rId1"/>
+    <sheet name="SYSC 4502" sheetId="2" r:id="rId2"/>
+    <sheet name="SYSC 4415" sheetId="3" r:id="rId3"/>
+    <sheet name="TSES 4012" sheetId="5" r:id="rId4"/>
+    <sheet name="SYSC 4602" sheetId="7" state="hidden" r:id="rId5"/>
+    <sheet name="ELEC 4705" sheetId="6" state="hidden" r:id="rId6"/>
+    <sheet name="SYSC 4310" sheetId="8" state="hidden" r:id="rId7"/>
+    <sheet name="SYSC4810" sheetId="9" state="hidden" r:id="rId8"/>
+    <sheet name="SYSC4805" sheetId="10" r:id="rId9"/>
+    <sheet name="SYSC 4907" sheetId="11" r:id="rId10"/>
+    <sheet name="Transcript" sheetId="14" r:id="rId11"/>
+    <sheet name="Sheet1" sheetId="15" state="hidden" r:id="rId12"/>
+    <sheet name="LetterGrade Lookup" sheetId="12" state="hidden" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="114">
   <si>
     <t>Deliverable Name</t>
   </si>
@@ -199,9 +198,6 @@
     <t>Labs</t>
   </si>
   <si>
-    <t>Project</t>
-  </si>
-  <si>
     <t>Assignments</t>
   </si>
   <si>
@@ -217,57 +213,15 @@
     <t>Project:</t>
   </si>
   <si>
-    <t>Iteration 1</t>
-  </si>
-  <si>
-    <t>Iteration 2</t>
-  </si>
-  <si>
-    <t>Iteration 3</t>
-  </si>
-  <si>
-    <t>Iteration 4</t>
-  </si>
-  <si>
-    <t>Iteration 5</t>
-  </si>
-  <si>
     <t>Project Final</t>
   </si>
   <si>
-    <t>Midterms:</t>
-  </si>
-  <si>
-    <t>Midterm Average</t>
-  </si>
-  <si>
-    <t>Oral</t>
-  </si>
-  <si>
-    <t>Written</t>
-  </si>
-  <si>
-    <t>Quizzes:</t>
-  </si>
-  <si>
-    <t>Test Average</t>
-  </si>
-  <si>
     <t>Projects:</t>
   </si>
   <si>
-    <t>Individual</t>
-  </si>
-  <si>
-    <t>Group</t>
-  </si>
-  <si>
     <t>Projects Average</t>
   </si>
   <si>
-    <t>Participation Submissions</t>
-  </si>
-  <si>
     <t>Week 1</t>
   </si>
   <si>
@@ -304,21 +258,6 @@
     <t>Participation Average</t>
   </si>
   <si>
-    <t>Book Assessment</t>
-  </si>
-  <si>
-    <t>SYSC 3303</t>
-  </si>
-  <si>
-    <t>SYSC 3320</t>
-  </si>
-  <si>
-    <t>SYSC 4001</t>
-  </si>
-  <si>
-    <t>SYSC 3501</t>
-  </si>
-  <si>
     <t>TSES 4012</t>
   </si>
   <si>
@@ -413,12 +352,51 @@
   </si>
   <si>
     <t>Lab 6</t>
+  </si>
+  <si>
+    <t>Grade</t>
+  </si>
+  <si>
+    <t>Midterms</t>
+  </si>
+  <si>
+    <t>SYSC 4504</t>
+  </si>
+  <si>
+    <t>Quizzes</t>
+  </si>
+  <si>
+    <t>SYSC 4415</t>
+  </si>
+  <si>
+    <t>SYSC 4502</t>
+  </si>
+  <si>
+    <t>Weekly Reflections</t>
+  </si>
+  <si>
+    <t>Week 13</t>
+  </si>
+  <si>
+    <t>Essay 1</t>
+  </si>
+  <si>
+    <t>Essay 2</t>
+  </si>
+  <si>
+    <t>Lecture Summary 1</t>
+  </si>
+  <si>
+    <t>Lecture Summary 2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -518,7 +496,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -548,6 +526,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
@@ -577,8 +558,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5DBE6C6A-8C2E-4294-82DF-56C65B6BCAF5}" name="Table2" displayName="Table2" ref="F5:H10" totalsRowShown="0">
-  <autoFilter ref="F5:H10" xr:uid="{FFE9CC18-36CC-4F13-886D-29DECCA1C422}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{5DBE6C6A-8C2E-4294-82DF-56C65B6BCAF5}" name="Table2" displayName="Table2" ref="F5:H9" totalsRowShown="0">
+  <autoFilter ref="F5:H9" xr:uid="{FFE9CC18-36CC-4F13-886D-29DECCA1C422}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{4B70864A-9E85-451B-8B76-02DAE33A2BDB}" name="Course"/>
     <tableColumn id="2" xr3:uid="{B65847F9-DCB2-4233-9A3C-9608CA24C62E}" name="Grade Percentage" dataDxfId="1"/>
@@ -889,7 +870,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -897,17 +878,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B40B08C-6FC0-4384-833D-8D5890E86605}">
-  <dimension ref="C2:H32"/>
+  <dimension ref="C2:H33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -918,7 +899,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>2</v>
@@ -930,323 +911,305 @@
     <row r="3" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="11" t="s">
-        <v>51</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.9</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F5" s="4">
         <f>D5*E5</f>
-        <v>1.8000000000000002E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>18</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.8</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ref="F6:F9" si="0">D6*E6</f>
-        <v>1.6E-2</v>
+        <f t="shared" ref="F6:F10" si="0">D6*E6</f>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.6</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
-        <v>1.2E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="4">
-        <v>0.8</v>
-      </c>
+        <v>11</v>
+      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>1.6E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="4">
-        <v>0.95</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="4">
-        <v>0.02</v>
+        <v>0.03</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
-        <v>1.9E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="14" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="F10" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="D10" s="4">
-        <f>AVERAGE(D5:D9)</f>
-        <v>0.81000000000000016</v>
-      </c>
-      <c r="E10" s="10">
-        <f>SUM(E5:E9)</f>
-        <v>0.1</v>
-      </c>
-      <c r="F10" s="4">
-        <f>SUM(F5:F9)</f>
-        <v>8.1000000000000003E-2</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0.08</v>
-      </c>
-      <c r="F13" s="4">
-        <f>D13*E13</f>
-        <v>7.2000000000000008E-2</v>
-      </c>
+      <c r="D11" s="4"/>
+      <c r="E11" s="10">
+        <f>SUM(E5:E10)</f>
+        <v>0.18</v>
+      </c>
+      <c r="F11" s="4">
+        <f>SUM(F5:F10)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D13" s="4"/>
     </row>
     <row r="14" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
-        <v>57</v>
-      </c>
-      <c r="D14" s="4">
-        <v>0.93799999999999994</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="D14" s="4"/>
       <c r="E14" s="4">
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" ref="F14:F17" si="1">D14*E14</f>
-        <v>7.5039999999999996E-2</v>
+        <f>D14*E14</f>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.85</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="D15" s="4"/>
       <c r="E15" s="4">
-        <v>0.08</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="1"/>
-        <v>6.8000000000000005E-2</v>
+        <f t="shared" ref="F15:F18" si="1">D15*E15</f>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>59</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="D16" s="4"/>
       <c r="E16" s="4">
-        <v>0.08</v>
+        <v>0.12</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>60</v>
-      </c>
-      <c r="D17" s="4">
-        <f>19.17/20</f>
-        <v>0.95850000000000013</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="4"/>
       <c r="E17" s="4">
-        <v>0.08</v>
+        <f>SUM(E14:E16)</f>
+        <v>0.22</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="1"/>
-        <v>7.6680000000000012E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C18" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="4">
-        <f>AVERAGE(D13:D17)</f>
-        <v>0.92930000000000013</v>
-      </c>
-      <c r="E18" s="4">
-        <f>SUM(E13:E17)</f>
-        <v>0.4</v>
-      </c>
-      <c r="F18" s="4">
-        <f>SUM(F13:F17)</f>
-        <v>0.37172000000000005</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>47</v>
-      </c>
-      <c r="D21" s="4">
-        <v>0.63</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="F21" s="4">
-        <f>D21*E21</f>
-        <v>6.3E-2</v>
-      </c>
+        <f>SUM(F14:F16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="4"/>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+    </row>
+    <row r="21" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="4"/>
     </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" s="4">
-        <v>1</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="D22" s="4"/>
       <c r="E22" s="4">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" ref="F22" si="2">D22*E22</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="23" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="4">
-        <f>AVERAGE(D21:D22)</f>
-        <v>0.81499999999999995</v>
-      </c>
-      <c r="E23" s="10">
-        <f>SUM(E21:E22)</f>
-        <v>0.2</v>
-      </c>
-      <c r="F23" s="4">
-        <f>SUM(F21:F22)</f>
-        <v>0.16300000000000001</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="14" t="s">
+        <f>D22*E22</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D23" s="4"/>
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>78</v>
+      </c>
+      <c r="D24" s="4"/>
+      <c r="E24" s="10">
+        <v>0.05</v>
+      </c>
+      <c r="F24" s="4">
+        <f>D24*E24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="E26" s="10">
-        <f>SUM(E18,E10,E23)</f>
-        <v>0.7</v>
-      </c>
-      <c r="F26" s="1">
-        <f>(SUM(F10,F18,F23)/E26)</f>
-        <v>0.87960000000000016</v>
-      </c>
-    </row>
-    <row r="27" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="11" t="s">
+      <c r="E27" s="10">
+        <f>SUM(E17,E11,E22,E24)</f>
+        <v>0.65000000000000013</v>
+      </c>
+      <c r="F27" s="1">
+        <f>(SUM(F11,F17,F24)/E27)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D28" s="4">
-        <v>0.95</v>
-      </c>
-      <c r="E28" s="4">
-        <f>1-E26</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="F28" s="4">
-        <f>D28*E28</f>
-        <v>0.28500000000000003</v>
-      </c>
-    </row>
-    <row r="29" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H29" s="12" t="s">
+      <c r="D29" s="4"/>
+      <c r="E29" s="4">
+        <f>1-E27</f>
+        <v>0.34999999999999987</v>
+      </c>
+      <c r="F29" s="4">
+        <f>D29*E29</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H30" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="14" t="s">
+    <row r="31" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C31" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E30" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F30" s="1">
-        <f>(F26*E26)+(D28*E28)</f>
-        <v>0.90072000000000008</v>
-      </c>
-      <c r="H30" t="str">
-        <f>LOOKUP(F30,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>A+</v>
-      </c>
-    </row>
-    <row r="31" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+      <c r="F31" s="1">
+        <f>(F27*E27)+(D29*E29)</f>
+        <v>0</v>
+      </c>
+      <c r="H31" t="str">
+        <f>LOOKUP(F31,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="32" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="10">
-        <v>0.95</v>
-      </c>
+      <c r="D33" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D12:D18 D7:D10">
+  <conditionalFormatting sqref="D7:D11 D13:D18">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="45"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D5:D6 D29 D21">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="45"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D11">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="45"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:D24">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1258,31 +1221,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D6 D28 D20">
-    <cfRule type="colorScale" priority="4">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="45"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D10">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="45"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D21:D23">
+  <conditionalFormatting sqref="D17">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -1300,269 +1239,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B801A28-B166-4E73-98CC-EEDEB78D5956}">
-  <dimension ref="B2:F21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>111</v>
-      </c>
-      <c r="C5" s="4">
-        <v>1</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E5" s="4">
-        <f>C5*D5</f>
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>112</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E6" s="4">
-        <f t="shared" ref="E6:E8" si="0">C6*D6</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.96</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="E7" s="4">
-        <f t="shared" si="0"/>
-        <v>0.192</v>
-      </c>
-    </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>113</v>
-      </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E8" s="4">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4">
-        <f>SUM(D5:D8)</f>
-        <v>0.5</v>
-      </c>
-      <c r="E9" s="4">
-        <f>SUM(E5:E8)</f>
-        <v>0.29200000000000004</v>
-      </c>
-    </row>
-    <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>114</v>
-      </c>
-      <c r="C12" s="4">
-        <v>0.73</v>
-      </c>
-      <c r="D12" s="4">
-        <v>0.05</v>
-      </c>
-      <c r="E12" s="4">
-        <f>C12*D12</f>
-        <v>3.6499999999999998E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>115</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0.91</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E13" s="4">
-        <f t="shared" ref="E13:E16" si="1">C13*D13</f>
-        <v>9.1000000000000011E-2</v>
-      </c>
-    </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>116</v>
-      </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="E14" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E15" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
-        <v>118</v>
-      </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4">
-        <v>0.1</v>
-      </c>
-      <c r="E16" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="10">
-        <f>SUM(D12:D16)</f>
-        <v>0.5</v>
-      </c>
-      <c r="E17" s="10">
-        <f>SUM(E12:E16)</f>
-        <v>0.1275</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="4">
-        <f>SUM(D17,D9)</f>
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <f>SUM(E9,E17)</f>
-        <v>0.41950000000000004</v>
-      </c>
-      <c r="F19" t="str">
-        <f>LOOKUP(E19,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>F</v>
-      </c>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
-        <v>45</v>
-      </c>
-      <c r="C21" s="10"/>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C5:C9 C11">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="30"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C12:C14 C16">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="30"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C15">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="30"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98FBC54-0CDF-4A45-9FE9-6E74382B401F}">
   <dimension ref="C25:F27"/>
   <sheetViews>
@@ -1593,12 +1269,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA2906D-355B-40D1-B17C-83040ED7030E}">
   <dimension ref="B4:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1607,17 +1283,17 @@
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.28515625" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="14" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="2:10" x14ac:dyDescent="0.25">
@@ -1628,7 +1304,7 @@
         <v>40</v>
       </c>
       <c r="D5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" t="s">
         <v>39</v>
@@ -1637,39 +1313,39 @@
         <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="J5" t="s">
-        <v>119</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C6" s="1">
         <f>SYSC4810!E23</f>
-        <v>0.47211253968253974</v>
+        <v>0.9271125396825397</v>
       </c>
       <c r="D6" t="str">
         <f>LOOKUP(C6,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>F</v>
+        <v>A+</v>
       </c>
       <c r="F6" t="s">
-        <v>86</v>
+        <v>104</v>
       </c>
       <c r="G6" s="1">
-        <f>'SYSC 3303'!F30</f>
-        <v>0.90072000000000008</v>
+        <f>'SYSC 4504'!F31</f>
+        <v>0</v>
       </c>
       <c r="H6" t="str">
         <f>LOOKUP(G6,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>A+</v>
+        <v>F</v>
       </c>
     </row>
     <row r="7" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="C7" s="1">
         <f>SYSC4805!E19</f>
@@ -1680,92 +1356,81 @@
         <v>F</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="G7" s="1">
-        <f>'SYSC 3320'!F19</f>
-        <v>0.8899999999999999</v>
+        <f>'SYSC 4502'!F27</f>
+        <v>0</v>
       </c>
       <c r="H7" t="str">
         <f>LOOKUP(G7,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>A</v>
+        <v>F</v>
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="C8" s="1">
-        <f>'ELEC 4705'!E21</f>
-        <v>0</v>
+        <f>'ELEC 4705'!C14</f>
+        <v>0.92</v>
       </c>
       <c r="D8" t="str">
         <f>LOOKUP(C8,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>F</v>
+        <v>A+</v>
       </c>
       <c r="F8" t="s">
-        <v>88</v>
+        <v>106</v>
       </c>
       <c r="G8" s="1">
-        <f>'SYSC 4001'!F20</f>
-        <v>0.83499999999999996</v>
+        <f>'SYSC 4415'!F24</f>
+        <v>0</v>
       </c>
       <c r="H8" t="str">
         <f>LOOKUP(G8,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>A-</v>
+        <v>F</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="C9" s="1">
         <f>'SYSC 4310'!E24</f>
-        <v>0.53964999999999996</v>
+        <v>0.93164999999999987</v>
       </c>
       <c r="D9" t="str">
         <f>LOOKUP(C9,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>D</v>
+        <v>A+</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>70</v>
       </c>
       <c r="G9" s="1">
-        <f>'SYSC 3501'!F24</f>
-        <v>0.84189999999999998</v>
+        <f>'TSES 4012'!F30</f>
+        <v>0</v>
       </c>
       <c r="H9" t="str">
         <f>LOOKUP(G9,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>A-</v>
+        <v>F</v>
       </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="C10" s="1">
         <f>'SYSC 4602'!E24</f>
-        <v>0.46899999999999997</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="D10" t="str">
         <f>LOOKUP(C10,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>F</v>
-      </c>
-      <c r="F10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G10" s="1">
-        <f>'TSES 4012'!F26</f>
-        <v>0.90199999999999991</v>
-      </c>
-      <c r="H10" t="str">
-        <f>LOOKUP(G10,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
         <v>A+</v>
       </c>
     </row>
     <row r="11" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="C11" s="1">
         <f>'SYSC 4907'!E25</f>
@@ -1785,7 +1450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE9BA02F-B7FA-49AA-81AC-14B83DC59856}">
   <dimension ref="B2:B29"/>
   <sheetViews>
@@ -1944,7 +1609,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA43BB96-763E-4471-A439-6E156A2AE051}">
   <dimension ref="B3:C15"/>
   <sheetViews>
@@ -2069,17 +1734,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F42871C-6C37-4276-988F-E0CB1B38DC91}">
-  <dimension ref="C2:H21"/>
+  <dimension ref="C2:H29"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -2090,7 +1755,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>1</v>
+        <v>102</v>
       </c>
       <c r="E2" s="12" t="s">
         <v>2</v>
@@ -2102,88 +1767,85 @@
     <row r="3" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4">
-        <v>1</v>
-      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="4">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F5" s="4">
         <f>D5*E5</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="4">
-        <v>1</v>
-      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="4">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F6" s="4">
         <f t="shared" ref="F6:F10" si="0">D6*E6</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F7" s="4">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="4">
-        <v>1</v>
-      </c>
+      <c r="D8" s="4"/>
       <c r="E8" s="4">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="4">
-        <v>1</v>
-      </c>
+      <c r="D9" s="4"/>
       <c r="E9" s="4">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="F9" s="4">
         <f t="shared" si="0"/>
-        <v>0.05</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>101</v>
+      </c>
       <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
+      <c r="E10" s="4">
+        <v>0.03</v>
+      </c>
       <c r="F10" s="4">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2193,99 +1855,163 @@
       <c r="C11" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="4">
-        <f>AVERAGE(D5:D10)</f>
-        <v>1</v>
-      </c>
+      <c r="D11" s="4"/>
       <c r="E11" s="4">
         <f>SUM(E5:E10)</f>
-        <v>0.25</v>
+        <v>0.18</v>
       </c>
       <c r="F11" s="4">
         <f>SUM(F5:F10)</f>
-        <v>0.25</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="13" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="4">
-        <v>0.88</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="F13" s="4">
-        <f>D13*E13</f>
-        <v>0.22</v>
-      </c>
-    </row>
-    <row r="15" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E15" s="10">
-        <f>SUM(E11,E13)</f>
-        <v>0.5</v>
-      </c>
-      <c r="F15" s="1">
-        <f>(SUM(F11,F13)/E15)</f>
-        <v>0.94</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C17" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.84</v>
-      </c>
-      <c r="E17" s="4">
-        <f>1-E15</f>
-        <v>0.5</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="E14" s="4">
+        <v>0.03</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" ref="F14:F17" si="1">D14*E14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C15" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C16" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" s="10">
+        <f>SUM(E14:E16)</f>
+        <v>0.15000000000000002</v>
       </c>
       <c r="F17" s="4">
-        <f>D17*E17</f>
-        <v>0.42</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H18" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C19" s="14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E19" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F19" s="1">
-        <f>(F15*E15)+(D17*E17)</f>
-        <v>0.8899999999999999</v>
-      </c>
-      <c r="H19" t="str">
-        <f>LOOKUP(F19,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>A</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <f>SUM(F14:F16)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+      <c r="E20" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F20" s="4">
+        <f>D19*E20</f>
+        <v>0</v>
+      </c>
+    </row>
     <row r="21" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
+        <v>48</v>
+      </c>
+      <c r="E21" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="F21" s="4">
+        <f>D20*E21</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="10">
+        <f>SUM(E11,E17,E20:E21)</f>
+        <v>0.73</v>
+      </c>
+      <c r="F23" s="1">
+        <f>(SUM(F11,F20)/E23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4">
+        <f>1-E23</f>
+        <v>0.27</v>
+      </c>
+      <c r="F25" s="4">
+        <f>D25*E25</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H26" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="1">
+        <f>(F23*E23)+(D25*E25)</f>
+        <v>0</v>
+      </c>
+      <c r="H27" t="str">
+        <f>LOOKUP(F27,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="28" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
         <v>45</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D29" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D4:D11">
+  <conditionalFormatting sqref="D5:D11">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2297,7 +2023,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D13 D17">
+  <conditionalFormatting sqref="D25 D19">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2315,10 +2041,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B24F5A-D51A-416E-8B54-9C8C94319869}">
-  <dimension ref="C2:H22"/>
+  <dimension ref="C2:H26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2348,198 +2074,217 @@
     <row r="3" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C4" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="4">
-        <v>0.91</v>
-      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F5" s="4">
         <f>D5*E5</f>
-        <v>9.1000000000000011E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="4">
-        <v>0.85</v>
-      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F6" s="4">
         <f>D6*E6</f>
-        <v>8.5000000000000006E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="4">
-        <v>1</v>
-      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="4">
-        <v>0.1</v>
+        <v>0.05</v>
       </c>
       <c r="F7" s="4">
         <f>D7*E7</f>
-        <v>0.1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F8" s="4">
+        <f>D8*E8</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="D8" s="4">
-        <f>AVERAGE(D5:D7)</f>
-        <v>0.91999999999999993</v>
-      </c>
-      <c r="E8" s="10">
-        <f>SUM(E5:E7)</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="F8" s="4">
+      <c r="D9" s="4"/>
+      <c r="E9" s="10">
+        <f>SUM(E5:E8)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F9" s="4">
         <f>SUM(F5:F7)</f>
-        <v>0.27600000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.67</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.2</v>
-      </c>
-      <c r="F10" s="4">
-        <f>D10*E10</f>
-        <v>0.13400000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="10">
-        <f>SUM(E8,E10)</f>
-        <v>0.5</v>
-      </c>
-      <c r="F12" s="1">
-        <f>(SUM(F8,F10)/E12)</f>
-        <v>0.82000000000000006</v>
-      </c>
-    </row>
-    <row r="14" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="4"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="11" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F12" s="4">
+        <f t="shared" ref="F12:F15" si="0">D12*E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>86</v>
+      </c>
       <c r="E14" s="4">
-        <f>1-E12</f>
-        <v>0.5</v>
-      </c>
-      <c r="F14" s="10">
-        <f>SUM(F15:F17)/E14</f>
-        <v>0.85</v>
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>50</v>
-      </c>
-      <c r="D15" s="4">
-        <v>0.85</v>
+        <v>87</v>
       </c>
       <c r="E15" s="4">
-        <v>0.3</v>
+        <v>0.05</v>
       </c>
       <c r="F15" s="4">
-        <f>D15*E15</f>
-        <v>0.255</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
+        <v>41</v>
       </c>
       <c r="E16" s="4">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F16" s="4">
         <f>D16*E16</f>
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>65</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.8</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0.15</v>
-      </c>
-      <c r="F17" s="4">
-        <f>D17*E17</f>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H19" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="F18" s="4">
+        <f>D18*E18</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C20" s="11" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="3" t="s">
+      <c r="E20" s="10">
+        <f>SUM(E9,E16,E18)</f>
+        <v>0.65</v>
+      </c>
+      <c r="F20" s="1">
+        <f>(SUM(F9,F18)/E20)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D22" s="4"/>
+      <c r="E22" s="4">
+        <f>1-E20</f>
+        <v>0.35</v>
+      </c>
+      <c r="F22" s="17"/>
+    </row>
+    <row r="23" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H23" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D24" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F20" s="1">
-        <f>(F12*E12)+(F14*E14)</f>
-        <v>0.83499999999999996</v>
-      </c>
-      <c r="H20" t="str">
-        <f>LOOKUP(F20,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>A-</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+      <c r="E24" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="1">
+        <f>(F20*E20)+(F22*E22)</f>
+        <v>0</v>
+      </c>
+      <c r="H24" t="str">
+        <f>LOOKUP(F24,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
         <v>45</v>
       </c>
-      <c r="D22" s="10"/>
+      <c r="D26" s="10"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D7">
+  <conditionalFormatting sqref="D7:D10 D18">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2551,7 +2296,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D6 D14 D8:D10">
+  <conditionalFormatting sqref="D5:D6 D22">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2563,7 +2308,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
+  <conditionalFormatting sqref="D9">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2580,24 +2325,24 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4102EE0F-DF8D-4EE5-96AB-54790ABFC13E}">
-  <dimension ref="C2:H26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2086A78-E6EF-4D16-A854-20A999490499}">
+  <dimension ref="B2:H30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C2" s="12" t="s">
         <v>0</v>
       </c>
@@ -2611,243 +2356,321 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="6"/>
       <c r="C4" s="11" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="3:6" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="6"/>
       <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.85</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="D5" s="4"/>
       <c r="E5" s="4">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="F5" s="4">
         <f>D5*E5</f>
-        <v>8.5000000000000006E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:6" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="7"/>
       <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="4">
-        <v>1.2</v>
-      </c>
+        <v>111</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="4">
         <v>0.1</v>
       </c>
       <c r="F6" s="4">
-        <f t="shared" ref="F6" si="0">D6*E6</f>
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="7" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C7" s="14" t="s">
-        <v>41</v>
+        <f t="shared" ref="F6:F8" si="0">D6*E6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="6"/>
+      <c r="C7" t="s">
+        <v>112</v>
       </c>
       <c r="D7" s="4"/>
       <c r="E7" s="10">
-        <f>SUM(E5:E6)</f>
-        <v>0.2</v>
+        <v>0.02</v>
       </c>
       <c r="F7" s="4">
-        <f>SUM(F5:F6)</f>
-        <v>0.20500000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C9" s="11" t="s">
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="6"/>
+      <c r="C8" t="s">
+        <v>113</v>
+      </c>
+      <c r="D8" s="4"/>
+      <c r="E8" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="F8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="6"/>
+      <c r="C9" s="14" t="s">
+        <v>57</v>
       </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
-        <v>5</v>
-      </c>
-      <c r="D10" s="4">
-        <v>0.63</v>
-      </c>
-      <c r="E10" s="4">
-        <v>0.25</v>
-      </c>
-      <c r="F10" s="4">
-        <f>D10*E10</f>
-        <v>0.1575</v>
-      </c>
-    </row>
-    <row r="11" spans="3:6" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
-        <v>6</v>
-      </c>
-      <c r="D11" s="4">
-        <v>0.86</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0.35</v>
-      </c>
-      <c r="F11" s="4">
-        <f>D11*E11</f>
-        <v>0.30099999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="10">
-        <f>SUM(E10:E11)</f>
-        <v>0.6</v>
+      <c r="E9" s="10">
+        <f>SUM(E5:E8)</f>
+        <v>0.34000000000000008</v>
+      </c>
+      <c r="F9" s="4">
+        <f>SUM(F5:F7)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="6"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="6"/>
+      <c r="C11" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="6"/>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="4"/>
+      <c r="E12" s="18">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F12" s="4">
-        <f>SUM(F10:F11)</f>
-        <v>0.45850000000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="11" t="s">
-        <v>7</v>
+        <f>D12*E12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C13" t="s">
+        <v>59</v>
+      </c>
+      <c r="D13" s="4"/>
+      <c r="E13" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F13" s="4">
+        <f t="shared" ref="F13:F22" si="1">D13*E13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C14" t="s">
+        <v>60</v>
       </c>
       <c r="D14" s="4"/>
-    </row>
-    <row r="15" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E14" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F14" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
-        <v>8</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0.04</v>
+        <v>61</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="18">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F15" s="4">
-        <f>D15*E15</f>
-        <v>0.04</v>
-      </c>
-    </row>
-    <row r="16" spans="3:6" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="4">
-        <v>0.92</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0.04</v>
+        <v>62</v>
+      </c>
+      <c r="D16" s="4"/>
+      <c r="E16" s="18">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" ref="F16:F19" si="1">D16*E16</f>
-        <v>3.6799999999999999E-2</v>
+        <f t="shared" si="1"/>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0.87</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0.04</v>
+        <v>63</v>
+      </c>
+      <c r="D17" s="4"/>
+      <c r="E17" s="18">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F17" s="4">
         <f t="shared" si="1"/>
-        <v>3.4799999999999998E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>11</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0.88</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0.04</v>
+        <v>64</v>
+      </c>
+      <c r="D18" s="4"/>
+      <c r="E18" s="18">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F18" s="4">
         <f t="shared" si="1"/>
-        <v>3.5200000000000002E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C19" t="s">
-        <v>12</v>
-      </c>
-      <c r="D19" s="4">
-        <v>0.79</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0.04</v>
+        <v>65</v>
+      </c>
+      <c r="D19" s="4"/>
+      <c r="E19" s="18">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F19" s="4">
         <f t="shared" si="1"/>
-        <v>3.1600000000000003E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C20" s="14" t="s">
-        <v>23</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>66</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="4">
-        <f>SUM(E15:E19)</f>
-        <v>0.2</v>
+      <c r="E20" s="18">
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="F20" s="4">
-        <f>SUM(F15:F19)</f>
-        <v>0.1784</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="4"/>
+      <c r="E21" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F21" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>68</v>
+      </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H23" s="12" t="s">
+      <c r="E22" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F22" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>109</v>
+      </c>
+      <c r="D23" s="4"/>
+      <c r="E23" s="18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F23" s="4">
+        <f t="shared" ref="F23" si="2">D23*E23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="19">
+        <f>SUM(E12:E23)</f>
+        <v>5.9999999999999991E-2</v>
+      </c>
+      <c r="F24" s="4">
+        <f>SUM(F12:F23)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="10">
+        <f>SUM(E9,E24)</f>
+        <v>0.40000000000000008</v>
+      </c>
+      <c r="F26" s="1">
+        <f>(SUM(F9,F24)/E26)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4">
+        <f>1-E26</f>
+        <v>0.59999999999999987</v>
+      </c>
+      <c r="F27" s="17"/>
+    </row>
+    <row r="29" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H29" s="12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="14" t="s">
+    <row r="30" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E30" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F24" s="1">
-        <f>F7+F12+F20</f>
-        <v>0.84189999999999998</v>
-      </c>
-      <c r="H24" t="str">
-        <f>LOOKUP(F24,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>A-</v>
-      </c>
-    </row>
-    <row r="25" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" s="10"/>
+      <c r="F30" s="1">
+        <f>SUM(F26,F27)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" t="str">
+        <f>LOOKUP(F30,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
+        <v>F</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D7 D20 D9 D14">
+  <conditionalFormatting sqref="D9:D24">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2859,19 +2682,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D6 D22">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="45"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D7">
+  <conditionalFormatting sqref="D9">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2883,7 +2694,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D10:D11">
+  <conditionalFormatting sqref="D5:D8">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2895,7 +2706,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D15:D19">
+  <conditionalFormatting sqref="D27">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2912,376 +2723,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2086A78-E6EF-4D16-A854-20A999490499}">
-  <dimension ref="B2:H26"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="9.140625" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C2" s="12" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="6"/>
-      <c r="C4" s="11" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="6"/>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.88</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F5" s="4">
-        <f>D5*E5</f>
-        <v>0.26400000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" s="7"/>
-      <c r="C6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.9</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.3</v>
-      </c>
-      <c r="F6" s="4">
-        <f t="shared" ref="F6:F7" si="0">D6*E6</f>
-        <v>0.27</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="6"/>
-      <c r="C7" t="s">
-        <v>85</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.94</v>
-      </c>
-      <c r="E7" s="10">
-        <v>0.2</v>
-      </c>
-      <c r="F7" s="4">
-        <f t="shared" si="0"/>
-        <v>0.188</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="6"/>
-      <c r="C8" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="D8" s="4"/>
-      <c r="E8" s="10">
-        <f>SUM(E5:E7)</f>
-        <v>0.8</v>
-      </c>
-      <c r="F8" s="4">
-        <f>SUM(F5:F7)</f>
-        <v>0.72199999999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-    </row>
-    <row r="10" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="6"/>
-      <c r="C10" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="6"/>
-      <c r="C11" t="s">
-        <v>73</v>
-      </c>
-      <c r="D11" s="4">
-        <v>1</v>
-      </c>
-      <c r="E11" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F11" s="4">
-        <f>D11*E11</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
-        <v>74</v>
-      </c>
-      <c r="D12" s="4">
-        <v>1</v>
-      </c>
-      <c r="E12" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F12" s="4">
-        <f t="shared" ref="F12:F21" si="1">D12*E12</f>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
-        <v>75</v>
-      </c>
-      <c r="D13" s="4">
-        <v>1</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F13" s="4">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
-        <v>76</v>
-      </c>
-      <c r="D14" s="4">
-        <v>1</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F14" s="4">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
-        <v>77</v>
-      </c>
-      <c r="D15" s="4">
-        <v>1</v>
-      </c>
-      <c r="E15" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F15" s="4">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
-        <v>78</v>
-      </c>
-      <c r="D16" s="4">
-        <v>1</v>
-      </c>
-      <c r="E16" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F16" s="4">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
-        <v>79</v>
-      </c>
-      <c r="D17" s="4">
-        <v>0</v>
-      </c>
-      <c r="E17" s="4">
-        <v>0</v>
-      </c>
-      <c r="F17" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
-        <v>80</v>
-      </c>
-      <c r="D18" s="4">
-        <v>0</v>
-      </c>
-      <c r="E18" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F18" s="4">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
-        <v>81</v>
-      </c>
-      <c r="D19" s="4">
-        <v>1</v>
-      </c>
-      <c r="E19" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F19" s="4">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
-        <v>82</v>
-      </c>
-      <c r="D20" s="4">
-        <v>1</v>
-      </c>
-      <c r="E20" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F20" s="4">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
-        <v>83</v>
-      </c>
-      <c r="D21" s="4">
-        <v>1</v>
-      </c>
-      <c r="E21" s="4">
-        <v>0.02</v>
-      </c>
-      <c r="F21" s="4">
-        <f t="shared" si="1"/>
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-    </row>
-    <row r="23" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="E23" s="10">
-        <f>SUM(E11:E21)</f>
-        <v>0.19999999999999998</v>
-      </c>
-      <c r="F23" s="4">
-        <f>SUM(F11:F21)</f>
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="24" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="H25" s="12" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="3:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="1">
-        <f>SUM(F8,F23)</f>
-        <v>0.90199999999999991</v>
-      </c>
-      <c r="H26" t="str">
-        <f>LOOKUP(F26,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>A+</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D8:D22">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="45"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D8">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="45"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D7">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="45"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D8DB95B-AC99-4DBB-8BA6-C9CFD039004E}">
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3309,12 +2755,12 @@
     <row r="3" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="11" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="C5" s="4">
         <v>1</v>
@@ -3329,7 +2775,7 @@
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="C6" s="4">
         <v>0.85</v>
@@ -3344,7 +2790,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4">
@@ -3448,7 +2894,7 @@
     </row>
     <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="C15" s="4">
         <v>1</v>
@@ -3464,7 +2910,7 @@
     </row>
     <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="C16" s="4"/>
       <c r="D16" s="4">
@@ -3525,14 +2971,16 @@
       <c r="B23" t="s">
         <v>13</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4">
+        <v>0.9</v>
+      </c>
       <c r="D23" s="4">
         <f>1-D21</f>
         <v>0.5</v>
       </c>
       <c r="E23" s="8">
         <f>C23*D23</f>
-        <v>0</v>
+        <v>0.45</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -3547,11 +2995,11 @@
       </c>
       <c r="E24" s="1">
         <f>(E21*D21)+(D23*C23)</f>
-        <v>0.46899999999999997</v>
+        <v>0.91900000000000004</v>
       </c>
       <c r="F24" t="str">
         <f>LOOKUP(E24,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>F</v>
+        <v>A+</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -3604,12 +3052,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23824A43-8FC1-46A6-857D-F140B2060BA9}">
   <dimension ref="B2:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3672,7 +3120,7 @@
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C7" s="4">
         <v>0.93</v>
@@ -3687,7 +3135,7 @@
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="C8" s="4">
         <v>0.91700000000000004</v>
@@ -3702,7 +3150,7 @@
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
@@ -3752,14 +3200,16 @@
       <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="4"/>
+      <c r="C14" s="4">
+        <v>0.92</v>
+      </c>
       <c r="D14" s="4">
         <f>1-D12</f>
         <v>0.5</v>
       </c>
       <c r="E14" s="8">
         <f>C14*D14</f>
-        <v>0</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.25">
@@ -3774,11 +3224,11 @@
       </c>
       <c r="E15" s="1">
         <f>(E12*D12)+(D14*C14)</f>
-        <v>0.47581249999999997</v>
+        <v>0.93581249999999994</v>
       </c>
       <c r="F15" t="str">
         <f>LOOKUP(E15,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>F</v>
+        <v>A+</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.25">
@@ -3844,12 +3294,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17383B8E-801E-49B3-80FC-FEE68206AB6A}">
   <dimension ref="B2:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3877,7 +3327,7 @@
     <row r="3" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -4016,7 +3466,7 @@
     </row>
     <row r="17" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B17" s="11" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.25">
@@ -4052,14 +3502,16 @@
       <c r="B22" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="4"/>
+      <c r="C22" s="4">
+        <v>0.98</v>
+      </c>
       <c r="D22" s="4">
         <f>1-D20</f>
         <v>0.39999999999999991</v>
       </c>
       <c r="E22">
         <f>C22*D22</f>
-        <v>0</v>
+        <v>0.3919999999999999</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.25">
@@ -4074,11 +3526,11 @@
       </c>
       <c r="E24" s="1">
         <f>(E20*D20)+(D22*C22)</f>
-        <v>0.53964999999999996</v>
+        <v>0.93164999999999987</v>
       </c>
       <c r="F24" t="str">
         <f>LOOKUP(E24,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>D</v>
+        <v>A+</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
@@ -4119,12 +3571,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DD28651-12EC-44C5-8BAE-83A80F2C299F}">
   <dimension ref="B2:F25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4189,7 +3641,7 @@
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>106</v>
+        <v>86</v>
       </c>
       <c r="C7" s="4">
         <v>1</v>
@@ -4205,7 +3657,7 @@
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="C8" s="4">
         <v>0.85</v>
@@ -4221,7 +3673,7 @@
     </row>
     <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="C9" s="4">
         <v>0.7142857142857143</v>
@@ -4248,7 +3700,7 @@
     </row>
     <row r="12" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
@@ -4321,7 +3773,7 @@
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>105</v>
+        <v>85</v>
       </c>
       <c r="C17" s="4">
         <v>1</v>
@@ -4368,14 +3820,16 @@
       <c r="B21" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="5"/>
+      <c r="C21" s="4">
+        <v>0.91</v>
+      </c>
       <c r="D21" s="4">
         <f>1-D20</f>
         <v>0.5</v>
       </c>
       <c r="E21" s="4">
         <f>C21*D21</f>
-        <v>0</v>
+        <v>0.45500000000000002</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
@@ -4391,11 +3845,11 @@
       <c r="D23" s="4"/>
       <c r="E23" s="1">
         <f>(E20*D20)+(C21*D21)</f>
-        <v>0.47211253968253974</v>
+        <v>0.9271125396825397</v>
       </c>
       <c r="F23" t="str">
         <f>LOOKUP(E23,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>F</v>
+        <v>A+</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.25">
@@ -4408,8 +3862,20 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C12:C18 C5:C9">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="C5:C9 C12:C18">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF00B050"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C21">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="50"/>
@@ -4422,4 +3888,267 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B801A28-B166-4E73-98CC-EEDEB78D5956}">
+  <dimension ref="B2:F21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:5" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="2:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="11" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C5" s="4">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E5" s="4">
+        <f>C5*D5</f>
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="4">
+        <f t="shared" ref="E6:E8" si="0">C6*D6</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4">
+        <v>0.96</v>
+      </c>
+      <c r="D7" s="4">
+        <v>0.2</v>
+      </c>
+      <c r="E7" s="4">
+        <f t="shared" si="0"/>
+        <v>0.192</v>
+      </c>
+    </row>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E8" s="4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4">
+        <f>SUM(D5:D8)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E9" s="4">
+        <f>SUM(E5:E8)</f>
+        <v>0.29200000000000004</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+    </row>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" s="4">
+        <v>0.73</v>
+      </c>
+      <c r="D12" s="4">
+        <v>0.05</v>
+      </c>
+      <c r="E12" s="4">
+        <f>C12*D12</f>
+        <v>3.6499999999999998E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C13" s="4">
+        <v>0.91</v>
+      </c>
+      <c r="D13" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E13" s="4">
+        <f t="shared" ref="E13:E16" si="1">C13*D13</f>
+        <v>9.1000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>96</v>
+      </c>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4">
+        <v>0.15</v>
+      </c>
+      <c r="E14" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E15" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>98</v>
+      </c>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4">
+        <v>0.1</v>
+      </c>
+      <c r="E16" s="4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D17" s="10">
+        <f>SUM(D12:D16)</f>
+        <v>0.5</v>
+      </c>
+      <c r="E17" s="10">
+        <f>SUM(E12:E16)</f>
+        <v>0.1275</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="4">
+        <f>SUM(D17,D9)</f>
+        <v>1</v>
+      </c>
+      <c r="E19" s="1">
+        <f>SUM(E9,E17)</f>
+        <v>0.41950000000000004</v>
+      </c>
+      <c r="F19" t="str">
+        <f>LOOKUP(E19,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="10"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="C5:C9 C11">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="30"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12:C14 C16">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="30"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C15">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="30"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated index html to include more structure Updated grades doc
</commit_message>
<xml_diff>
--- a/Year 4 Grades.xlsx
+++ b/Year 4 Grades.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\University\Year 4\Code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\University\4th_Year\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D082FC1B-73E1-4252-9252-722FEC9A977F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EED9E0FB-3BE7-4249-90E8-EEDBFDAC03F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8745" yWindow="7950" windowWidth="18060" windowHeight="15435" tabRatio="769" activeTab="2" xr2:uid="{A1BD24B9-1795-480B-9592-5AE2E18FE68C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="769" activeTab="1" xr2:uid="{A1BD24B9-1795-480B-9592-5AE2E18FE68C}"/>
   </bookViews>
   <sheets>
     <sheet name="SYSC 4504" sheetId="1" r:id="rId1"/>
@@ -496,7 +496,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -526,7 +526,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -881,7 +880,7 @@
   <dimension ref="C2:H33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1038,7 +1037,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" ref="F15:F18" si="1">D15*E15</f>
+        <f t="shared" ref="F15:F16" si="1">D15*E15</f>
         <v>0</v>
       </c>
     </row>
@@ -1360,7 +1359,7 @@
       </c>
       <c r="G7" s="1">
         <f>'SYSC 4502'!F27</f>
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H7" t="str">
         <f>LOOKUP(G7,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
@@ -1736,8 +1735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F42871C-6C37-4276-988F-E0CB1B38DC91}">
   <dimension ref="C2:H29"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1777,13 +1776,15 @@
       <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4">
+        <v>1</v>
+      </c>
       <c r="E5" s="4">
         <v>0.03</v>
       </c>
       <c r="F5" s="4">
         <f>D5*E5</f>
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
@@ -1862,7 +1863,7 @@
       </c>
       <c r="F11" s="4">
         <f>SUM(F5:F10)</f>
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="12" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1879,7 +1880,7 @@
         <v>0.03</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" ref="F14:F17" si="1">D14*E14</f>
+        <f t="shared" ref="F14:F16" si="1">D14*E14</f>
         <v>0</v>
       </c>
     </row>
@@ -1960,7 +1961,7 @@
       </c>
       <c r="F23" s="1">
         <f>(SUM(F11,F20)/E23)</f>
-        <v>0</v>
+        <v>4.1095890410958902E-2</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1995,7 +1996,7 @@
       </c>
       <c r="F27" s="1">
         <f>(F23*E23)+(D25*E25)</f>
-        <v>0</v>
+        <v>0.03</v>
       </c>
       <c r="H27" t="str">
         <f>LOOKUP(F27,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
@@ -2023,7 +2024,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D25 D19">
+  <conditionalFormatting sqref="D19 D25">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -2043,8 +2044,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B24F5A-D51A-416E-8B54-9C8C94319869}">
   <dimension ref="C2:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:F20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,7 +2251,6 @@
         <f>1-E20</f>
         <v>0.35</v>
       </c>
-      <c r="F22" s="17"/>
     </row>
     <row r="23" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H23" s="12" t="s">
@@ -2452,7 +2452,7 @@
         <v>58</v>
       </c>
       <c r="D12" s="4"/>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F12" s="4">
@@ -2465,7 +2465,7 @@
         <v>59</v>
       </c>
       <c r="D13" s="4"/>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F13" s="4">
@@ -2478,7 +2478,7 @@
         <v>60</v>
       </c>
       <c r="D14" s="4"/>
-      <c r="E14" s="18">
+      <c r="E14" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F14" s="4">
@@ -2491,7 +2491,7 @@
         <v>61</v>
       </c>
       <c r="D15" s="4"/>
-      <c r="E15" s="18">
+      <c r="E15" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F15" s="4">
@@ -2504,7 +2504,7 @@
         <v>62</v>
       </c>
       <c r="D16" s="4"/>
-      <c r="E16" s="18">
+      <c r="E16" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F16" s="4">
@@ -2517,7 +2517,7 @@
         <v>63</v>
       </c>
       <c r="D17" s="4"/>
-      <c r="E17" s="18">
+      <c r="E17" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F17" s="4">
@@ -2530,7 +2530,7 @@
         <v>64</v>
       </c>
       <c r="D18" s="4"/>
-      <c r="E18" s="18">
+      <c r="E18" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F18" s="4">
@@ -2543,7 +2543,7 @@
         <v>65</v>
       </c>
       <c r="D19" s="4"/>
-      <c r="E19" s="18">
+      <c r="E19" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F19" s="4">
@@ -2556,7 +2556,7 @@
         <v>66</v>
       </c>
       <c r="D20" s="4"/>
-      <c r="E20" s="18">
+      <c r="E20" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F20" s="4">
@@ -2569,7 +2569,7 @@
         <v>67</v>
       </c>
       <c r="D21" s="4"/>
-      <c r="E21" s="18">
+      <c r="E21" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F21" s="4">
@@ -2582,7 +2582,7 @@
         <v>68</v>
       </c>
       <c r="D22" s="4"/>
-      <c r="E22" s="18">
+      <c r="E22" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F22" s="4">
@@ -2595,7 +2595,7 @@
         <v>109</v>
       </c>
       <c r="D23" s="4"/>
-      <c r="E23" s="18">
+      <c r="E23" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F23" s="4">
@@ -2607,7 +2607,7 @@
       <c r="C24" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="19">
+      <c r="E24" s="18">
         <f>SUM(E12:E23)</f>
         <v>5.9999999999999991E-2</v>
       </c>
@@ -2642,7 +2642,6 @@
         <f>1-E26</f>
         <v>0.59999999999999987</v>
       </c>
-      <c r="F27" s="17"/>
     </row>
     <row r="29" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H29" s="12" t="s">

</xml_diff>

<commit_message>
Updated grades, cover letter
</commit_message>
<xml_diff>
--- a/Year 4 Grades.xlsx
+++ b/Year 4 Grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\University\4th_Year\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE2FBD4-2F28-4F16-9355-EA8A36F2912D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2C6BD2-28F8-408A-BF41-F9280166530D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="769" activeTab="10" xr2:uid="{A1BD24B9-1795-480B-9592-5AE2E18FE68C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="769" activeTab="2" xr2:uid="{A1BD24B9-1795-480B-9592-5AE2E18FE68C}"/>
   </bookViews>
   <sheets>
     <sheet name="SYSC 4504" sheetId="1" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="113">
   <si>
     <t>Deliverable Name</t>
   </si>
@@ -493,7 +493,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -524,7 +524,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
@@ -884,7 +883,7 @@
   <cols>
     <col min="2" max="2" width="9.140625" customWidth="1"/>
     <col min="3" max="3" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" customWidth="1"/>
     <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
@@ -992,13 +991,15 @@
       <c r="C10" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="4"/>
+      <c r="D10" s="4">
+        <v>1</v>
+      </c>
       <c r="E10" s="4">
         <v>0.03</v>
       </c>
       <c r="F10" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="11" spans="3:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1012,7 +1013,7 @@
       </c>
       <c r="F11" s="4">
         <f>SUM(F5:F10)</f>
-        <v>0.14400000000000002</v>
+        <v>0.17400000000000002</v>
       </c>
     </row>
     <row r="12" spans="3:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1136,7 +1137,7 @@
       </c>
       <c r="F27" s="1">
         <f>(SUM(F11,F17,F24,F22)/E27)</f>
-        <v>0.61553846153846148</v>
+        <v>0.66169230769230758</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1171,7 +1172,7 @@
       </c>
       <c r="F31" s="1">
         <f>(F27*E27)+(D29*E29)</f>
-        <v>0.40010000000000007</v>
+        <v>0.43010000000000004</v>
       </c>
       <c r="H31" t="str">
         <f>LOOKUP(F31,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
@@ -1183,12 +1184,14 @@
       <c r="C33" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="10">
+        <v>0.86</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D7:D11 D13:D18">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="D5:D6 D29 D21">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="45"/>
@@ -1199,8 +1202,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D6 D29 D21">
-    <cfRule type="colorScale" priority="5">
+  <conditionalFormatting sqref="D7:D11 D13:D18">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="45"/>
@@ -1223,8 +1226,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D22:D24">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="D17">
+    <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="45"/>
@@ -1235,8 +1238,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D17">
-    <cfRule type="colorScale" priority="1">
+  <conditionalFormatting sqref="D22:D24">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="45"/>
@@ -1287,8 +1290,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CA2906D-355B-40D1-B17C-83040ED7030E}">
   <dimension ref="B4:H11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,7 +1350,7 @@
       </c>
       <c r="G6" s="1">
         <f>'SYSC 4504'!F31</f>
-        <v>0.40010000000000007</v>
+        <v>0.43010000000000004</v>
       </c>
       <c r="H6" t="str">
         <f>LOOKUP(G6,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
@@ -1371,11 +1374,11 @@
       </c>
       <c r="G7" s="1">
         <f>'SYSC 4502'!F27</f>
-        <v>0.64114285714285724</v>
+        <v>0.67614285714285716</v>
       </c>
       <c r="H7" t="str">
         <f>LOOKUP(G7,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>C</v>
+        <v>C+</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
@@ -1395,11 +1398,11 @@
       </c>
       <c r="G8" s="1">
         <f>'SYSC 4415'!F31</f>
-        <v>0.52165833333333333</v>
+        <v>0.9139250000000001</v>
       </c>
       <c r="H8" t="str">
         <f>LOOKUP(G8,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>D-</v>
+        <v>A+</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
@@ -1419,7 +1422,7 @@
       </c>
       <c r="G9" s="1">
         <f>'ECOR 4995'!F30</f>
-        <v>0.35100000000000003</v>
+        <v>0.37600000000000006</v>
       </c>
       <c r="H9" t="str">
         <f>LOOKUP(G9,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
@@ -1749,7 +1752,7 @@
   <dimension ref="C2:H29"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,14 +1936,14 @@
         <v>19</v>
       </c>
       <c r="D16" s="4">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E16" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" si="1"/>
-        <v>3.5000000000000003E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="17" spans="3:8" x14ac:dyDescent="0.25">
@@ -1954,7 +1957,7 @@
       </c>
       <c r="F17" s="4">
         <f>SUM(F14:F16)</f>
-        <v>0.10400000000000001</v>
+        <v>0.13900000000000001</v>
       </c>
     </row>
     <row r="18" spans="3:8" x14ac:dyDescent="0.25">
@@ -2007,7 +2010,7 @@
       </c>
       <c r="F23" s="1">
         <f>(SUM(F11,F17,F20:F21)/E23)</f>
-        <v>0.87827788649706473</v>
+        <v>0.92622309197651664</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2043,11 +2046,11 @@
       </c>
       <c r="F27" s="1">
         <f>(F23*E23)+(D25*E25)</f>
-        <v>0.64114285714285724</v>
+        <v>0.67614285714285716</v>
       </c>
       <c r="H27" t="str">
         <f>LOOKUP(F27,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>C</v>
+        <v>C+</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2055,7 +2058,9 @@
       <c r="C29" t="s">
         <v>45</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10">
+        <v>0.83</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2071,8 +2076,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D19">
-    <cfRule type="colorScale" priority="6">
+  <conditionalFormatting sqref="D5:D21">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="45"/>
@@ -2083,8 +2088,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D21">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="D19">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="45"/>
@@ -2127,8 +2132,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B24F5A-D51A-416E-8B54-9C8C94319869}">
   <dimension ref="C2:H33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G46" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2169,12 +2174,11 @@
         <v>0.96</v>
       </c>
       <c r="E5" s="4">
-        <f>$E$8/3</f>
-        <v>6.6666666666666666E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F5" s="4">
         <f>D5*E5</f>
-        <v>6.4000000000000001E-2</v>
+        <v>5.7599999999999998E-2</v>
       </c>
     </row>
     <row r="6" spans="3:6" x14ac:dyDescent="0.25">
@@ -2185,26 +2189,26 @@
         <v>0.8</v>
       </c>
       <c r="E6" s="4">
-        <f t="shared" ref="E6:E7" si="0">$E$8/3</f>
-        <v>6.6666666666666666E-2</v>
+        <v>0.06</v>
       </c>
       <c r="F6" s="4">
         <f>D6*E6</f>
-        <v>5.3333333333333337E-2</v>
+        <v>4.8000000000000001E-2</v>
       </c>
     </row>
     <row r="7" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="4"/>
+      <c r="D7" s="4">
+        <v>1</v>
+      </c>
       <c r="E7" s="4">
-        <f t="shared" si="0"/>
-        <v>6.6666666666666666E-2</v>
+        <v>0.08</v>
       </c>
       <c r="F7" s="4">
         <f>D7*E7</f>
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="8" spans="3:6" x14ac:dyDescent="0.25">
@@ -2218,7 +2222,7 @@
       </c>
       <c r="F8" s="4">
         <f>SUM(F5:F7)</f>
-        <v>0.11733333333333335</v>
+        <v>0.18559999999999999</v>
       </c>
     </row>
     <row r="9" spans="3:6" x14ac:dyDescent="0.25">
@@ -2243,7 +2247,7 @@
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F11" s="4">
-        <f t="shared" ref="F11:F22" si="1">D11*E11</f>
+        <f t="shared" ref="F11:F22" si="0">D11*E11</f>
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
@@ -2255,11 +2259,11 @@
         <v>1</v>
       </c>
       <c r="E12" s="4">
-        <f t="shared" ref="E12:E22" si="2">$E$23/12</f>
+        <f t="shared" ref="E12:E22" si="1">$E$23/12</f>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F12" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
@@ -2271,11 +2275,11 @@
         <v>1</v>
       </c>
       <c r="E13" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F13" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
@@ -2287,11 +2291,11 @@
         <v>0.88</v>
       </c>
       <c r="E14" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F14" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4666666666666666E-2</v>
       </c>
     </row>
@@ -2303,11 +2307,11 @@
         <v>0.88</v>
       </c>
       <c r="E15" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F15" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4666666666666666E-2</v>
       </c>
     </row>
@@ -2323,7 +2327,7 @@
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="F16" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
@@ -2339,7 +2343,7 @@
         <v>8.3333333333333332E-3</v>
       </c>
       <c r="F17" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
@@ -2351,11 +2355,11 @@
         <v>0.88</v>
       </c>
       <c r="E18" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F18" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4666666666666666E-2</v>
       </c>
     </row>
@@ -2367,11 +2371,11 @@
         <v>0.75</v>
       </c>
       <c r="E19" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F19" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
@@ -2383,11 +2387,11 @@
         <v>0.88</v>
       </c>
       <c r="E20" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F20" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4666666666666666E-2</v>
       </c>
     </row>
@@ -2399,11 +2403,11 @@
         <v>0.88</v>
       </c>
       <c r="E21" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F21" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.4666666666666666E-2</v>
       </c>
     </row>
@@ -2415,11 +2419,11 @@
         <v>1</v>
       </c>
       <c r="E22" s="4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6666666666666666E-2</v>
       </c>
       <c r="F22" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
@@ -2428,14 +2432,14 @@
         <v>41</v>
       </c>
       <c r="D23" s="4">
-        <v>0.92</v>
+        <v>0.93</v>
       </c>
       <c r="E23" s="4">
         <v>0.2</v>
       </c>
       <c r="F23" s="4">
         <f>D23*E23</f>
-        <v>0.18400000000000002</v>
+        <v>0.18600000000000003</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2466,14 +2470,16 @@
       </c>
       <c r="F27" s="1">
         <f>(SUM(F8,F25,F23)/E27)</f>
-        <v>0.80255128205128201</v>
+        <v>0.91065384615384615</v>
       </c>
     </row>
     <row r="29" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="4">
+        <v>0.92</v>
+      </c>
       <c r="E29" s="4">
         <f>1-E27</f>
         <v>0.35</v>
@@ -2499,18 +2505,20 @@
       </c>
       <c r="F31" s="1">
         <f>(F27*E27)+(D29*E29)</f>
-        <v>0.52165833333333333</v>
+        <v>0.9139250000000001</v>
       </c>
       <c r="H31" t="str">
         <f>LOOKUP(F31,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>D-</v>
+        <v>A+</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
         <v>45</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="10">
+        <v>0.89</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2568,10 +2576,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2086A78-E6EF-4D16-A854-20A999490499}">
-  <dimension ref="B2:H30"/>
+  <dimension ref="B2:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2658,13 +2666,15 @@
       <c r="C8" t="s">
         <v>110</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
       <c r="E8" s="10">
         <v>0.02</v>
       </c>
       <c r="F8" s="4">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="9" spans="2:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2678,8 +2688,8 @@
         <v>0.34000000000000008</v>
       </c>
       <c r="F9" s="4">
-        <f>SUM(F5:F7)</f>
-        <v>0.29600000000000004</v>
+        <f>SUM(F5:F8)</f>
+        <v>0.31600000000000006</v>
       </c>
     </row>
     <row r="10" spans="2:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -2864,26 +2874,28 @@
       <c r="C23" t="s">
         <v>68</v>
       </c>
-      <c r="D23" s="4"/>
+      <c r="D23" s="4">
+        <v>1</v>
+      </c>
       <c r="E23" s="17">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="F23" s="4">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
     <row r="24" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="18">
+      <c r="E24" s="10">
         <f>SUM(E12:E23)</f>
         <v>5.9999999999999991E-2</v>
       </c>
       <c r="F24" s="4">
         <f>SUM(F12:F23)</f>
-        <v>5.4999999999999993E-2</v>
+        <v>5.9999999999999991E-2</v>
       </c>
     </row>
     <row r="25" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -2900,7 +2912,7 @@
       </c>
       <c r="F26" s="1">
         <f>(SUM(F9,F24)/E26)</f>
-        <v>0.87749999999999995</v>
+        <v>0.94</v>
       </c>
     </row>
     <row r="27" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2912,6 +2924,7 @@
         <f>1-E26</f>
         <v>0.59999999999999987</v>
       </c>
+      <c r="F27" s="1"/>
     </row>
     <row r="29" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
       <c r="H29" s="12" t="s">
@@ -2929,18 +2942,45 @@
         <v>16</v>
       </c>
       <c r="F30" s="1">
-        <f>SUM(F26*E26,F27*E27)</f>
-        <v>0.35100000000000003</v>
+        <f>SUM(F26*E26,D27*E27)</f>
+        <v>0.37600000000000006</v>
       </c>
       <c r="H30" t="str">
         <f>LOOKUP(F30,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
         <v>F</v>
       </c>
     </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>45</v>
+      </c>
+      <c r="D32" s="4">
+        <v>0.88</v>
+      </c>
+      <c r="E32" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="33" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D33" s="10">
+        <v>0.79</v>
+      </c>
+      <c r="E33" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="34" spans="4:5" x14ac:dyDescent="0.25">
+      <c r="D34" s="10">
+        <v>0.71</v>
+      </c>
+      <c r="E34" t="s">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D9:D24">
-    <cfRule type="colorScale" priority="3">
+  <conditionalFormatting sqref="D5:D8">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="45"/>
@@ -2963,8 +3003,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D5:D8">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="D9:D24">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="45"/>
@@ -3281,8 +3321,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="C23">
-    <cfRule type="colorScale" priority="2">
+  <conditionalFormatting sqref="C5:C8 C10:C16">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percent" val="50"/>
@@ -3305,8 +3345,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C5:C8 C10:C16">
-    <cfRule type="colorScale" priority="12">
+  <conditionalFormatting sqref="C23">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percent" val="50"/>
@@ -3535,24 +3575,24 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C14">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percent" val="50"/>
+        <cfvo type="percent" val="100"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C18">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="45"/>
         <cfvo type="num" val="1"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C14">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percent" val="50"/>
-        <cfvo type="percent" val="100"/>
         <color rgb="FFF8696B"/>
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>

</xml_diff>

<commit_message>
Added Kayla help code, resume updates
</commit_message>
<xml_diff>
--- a/Year 4 Grades.xlsx
+++ b/Year 4 Grades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="N:\University\4th_Year\Code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED2C6BD2-28F8-408A-BF41-F9280166530D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AE2670-EDF7-454A-B5F2-CB2893F644CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="769" activeTab="2" xr2:uid="{A1BD24B9-1795-480B-9592-5AE2E18FE68C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="769" xr2:uid="{A1BD24B9-1795-480B-9592-5AE2E18FE68C}"/>
   </bookViews>
   <sheets>
     <sheet name="SYSC 4504" sheetId="1" r:id="rId1"/>
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B40B08C-6FC0-4384-833D-8D5890E86605}">
   <dimension ref="C2:H33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1042,26 +1042,30 @@
       <c r="C15" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4">
+        <v>0.67</v>
+      </c>
       <c r="E15" s="4">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="F15" s="4">
         <f>D15*E15</f>
-        <v>0</v>
+        <v>4.6900000000000004E-2</v>
       </c>
     </row>
     <row r="16" spans="3:6" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>19</v>
       </c>
-      <c r="D16" s="4"/>
+      <c r="D16" s="4">
+        <v>0.92</v>
+      </c>
       <c r="E16" s="4">
         <v>0.12</v>
       </c>
       <c r="F16" s="4">
         <f t="shared" ref="F16" si="1">D16*E16</f>
-        <v>0</v>
+        <v>0.1104</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1075,7 +1079,7 @@
       </c>
       <c r="F17" s="4">
         <f>SUM(F14:F16)</f>
-        <v>2.76E-2</v>
+        <v>0.18490000000000001</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -1137,7 +1141,7 @@
       </c>
       <c r="F27" s="1">
         <f>(SUM(F11,F17,F24,F22)/E27)</f>
-        <v>0.66169230769230758</v>
+        <v>0.90369230769230757</v>
       </c>
     </row>
     <row r="28" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1145,14 +1149,16 @@
       <c r="C29" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="4"/>
+      <c r="D29" s="4">
+        <v>0.46</v>
+      </c>
       <c r="E29" s="4">
         <f>1-E27</f>
         <v>0.34999999999999987</v>
       </c>
       <c r="F29" s="4">
         <f>D29*E29</f>
-        <v>0</v>
+        <v>0.16099999999999995</v>
       </c>
     </row>
     <row r="30" spans="3:8" ht="18" thickBot="1" x14ac:dyDescent="0.35">
@@ -1172,11 +1178,11 @@
       </c>
       <c r="F31" s="1">
         <f>(F27*E27)+(D29*E29)</f>
-        <v>0.43010000000000004</v>
+        <v>0.74839999999999995</v>
       </c>
       <c r="H31" t="str">
         <f>LOOKUP(F31,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>F</v>
+        <v>B</v>
       </c>
     </row>
     <row r="32" spans="3:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
@@ -1350,11 +1356,11 @@
       </c>
       <c r="G6" s="1">
         <f>'SYSC 4504'!F31</f>
-        <v>0.43010000000000004</v>
+        <v>0.74839999999999995</v>
       </c>
       <c r="H6" t="str">
         <f>LOOKUP(G6,'LetterGrade Lookup'!B3:C15,'LetterGrade Lookup'!C3:C15)</f>
-        <v>F</v>
+        <v>B</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
@@ -2132,8 +2138,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{86B24F5A-D51A-416E-8B54-9C8C94319869}">
   <dimension ref="C2:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G46" sqref="A1:XFD1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>